<commit_message>
translations fixes, new data
</commit_message>
<xml_diff>
--- a/i18n/pl.xlsx
+++ b/i18n/pl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Birds" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Other" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Other" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="ExternalData_1" vbProcedure="false">Birds!$A$1:$G$357</definedName>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Ptaki obdarzone tą zdolnością znane są z przechowywania pożywienia na później. Zdolność ta pozwala przechować (położyć na karcie ptaka) 1 żeton pożywienia podczas każdej aktywacji tej karty. Przechowywane na karcie żetony nie mogą zostać wykorzystane w trakcie gry. Każdy z tych żetonów jest wart 1 punkt na koniec gry.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Avocet </t>
+    <t xml:space="preserve">American Avocet</t>
   </si>
   <si>
     <t xml:space="preserve">Recurvirostra americana</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">American Bittern </t>
+    <t xml:space="preserve">American Bittern</t>
   </si>
   <si>
     <t xml:space="preserve">Botaurus lentiginosus</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Pod karty tych ptaków możesz wsunąć kartę z ręki. Na koniec gry za każdą wsuniętą kartę otrzymasz 1 punkt. Dodatkowo karty ptaków z tej grupy oferują jeszcze jakąś korzyść (złożenie jaja, dobranie karty, zdobycie pożywienia). Możesz z niej skorzystać tylko wtedy, gdy najpierw wsunąłeś kartę z ręki pod tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Crow </t>
+    <t xml:space="preserve">American Crow</t>
   </si>
   <si>
     <t xml:space="preserve">Corvus brachyrhynchos</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">Te gatunki znane są z podjadania jaj z gniazd innych ptaków. Aby użyć tej zdolności, musisz mieć już złożone wcześniej jajo na innym ptaku. Odrzuć jajo do zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Goldfinch </t>
+    <t xml:space="preserve">American Goldfinch</t>
   </si>
   <si>
     <t xml:space="preserve">Spinus tristis</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Weź 3 [seed] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Kestrel </t>
+    <t xml:space="preserve">American Kestrel</t>
   </si>
   <si>
     <t xml:space="preserve">Falco sparverius</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">Drozd Wędrowny</t>
   </si>
   <si>
-    <t xml:space="preserve">American White Pelican </t>
+    <t xml:space="preserve">American White Pelican</t>
   </si>
   <si>
     <t xml:space="preserve">Pelecanus erythrorhynchos</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">Rzuć wszystkimi kośćmi znajdującymi się poza karmnikiem. Jeśli choć 1 kość wskaże [fish], weź 1 [fish] i przechowaj na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Anna's Hummingbird </t>
+    <t xml:space="preserve">Anna's Hummingbird</t>
   </si>
   <si>
     <t xml:space="preserve">Calypte anna</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">Właściciel kolibra decyduje, kto otrzymuje pożywienie jako pierwszy, a następnie obowiązuje kolejność rozgrywania. Gracze mogą napełniać karmnik, gdy opustoszeje, a także gdy wszystkie kości wskazują ten sam symbol (dotyczy także pojedynczej kostki).</t>
   </si>
   <si>
-    <t xml:space="preserve">Ash-Throated Flycatcher </t>
+    <t xml:space="preserve">Ash-Throated Flycatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Myiarchus cinerascens</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">Dobierz 2 [card] ze stosu. Wsuń 1 z nich pod tę kartę i zatrzymaj drugą.</t>
   </si>
   <si>
-    <t xml:space="preserve">Baird's Sparrow </t>
+    <t xml:space="preserve">Baird's Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Ammodramus bairdii</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">Złóż 1 [egg] i połóż na swojej dowolnej karcie ptaka.</t>
   </si>
   <si>
-    <t xml:space="preserve">Bald Eagle </t>
+    <t xml:space="preserve">Bald Eagle</t>
   </si>
   <si>
     <t xml:space="preserve">Haliaeetus leucocephalus</t>
@@ -328,7 +328,7 @@
     <t xml:space="preserve">Weź wszystkie [fish] z karmnika.</t>
   </si>
   <si>
-    <t xml:space="preserve">Baltimore Oriole </t>
+    <t xml:space="preserve">Baltimore Oriole</t>
   </si>
   <si>
     <t xml:space="preserve">Icterus galbula</t>
@@ -373,7 +373,7 @@
     <t xml:space="preserve">Te ptaki żywią się innymi ptakami. Porównaj rozpiętość skrzydeł wierzchniej karty ze stosu ze zdolnością drapieżnika.&lt;br&gt;Jeśli rozpiętość skrzydeł na wierzchniej karcie ze stosu jest mniejsza od limitu zdolności drapieżnika, wsuń tę kartę pod swoją kartę, aby zaznaczyć, że Twój drapieżnik skutecznie zapolował. Na koniec gry każda taka wsunięta karta warta jest 1 punkt.&lt;br&gt;Jeśli rozpiętość skrzydeł wierzchniej karty jest równa lub większa od zdolności Twojego drapieżnika, odrzuć ją.</t>
   </si>
   <si>
-    <t xml:space="preserve">Barrow's Goldeneye </t>
+    <t xml:space="preserve">Barrow's Goldeneye</t>
   </si>
   <si>
     <t xml:space="preserve">Bucephala islandica</t>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">Wireonek Skromny</t>
   </si>
   <si>
-    <t xml:space="preserve">Belted Kingfisher </t>
+    <t xml:space="preserve">Belted Kingfisher</t>
   </si>
   <si>
     <t xml:space="preserve">Megaceryle alcyon</t>
@@ -436,7 +436,7 @@
     <t xml:space="preserve">Wybierz siedlisko bez żadnych [egg]. Złóż 1 [egg] na każdej karcie w tym siedlisku.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black Skimmer </t>
+    <t xml:space="preserve">Black Skimmer</t>
   </si>
   <si>
     <t xml:space="preserve">Rynchops niger</t>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">Ta zdolność pozwala dobrać dodatkowe karty ptaków podczas wykonywania akcji „Dobierz karty ptaków”, ale ma swój koszt (odrzucenie karty). Gdy zastanawiasz się, którą kartę odrzucić, kolejny gracz może zacząć swoją turę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black Vulture </t>
+    <t xml:space="preserve">Black Vulture</t>
   </si>
   <si>
     <t xml:space="preserve">Coragyps atratus</t>
@@ -502,7 +502,7 @@
     <t xml:space="preserve">Odrzuć 1 [seed], aby wsunąć 2 [card] ze stosu pod tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black-Billed Magpie </t>
+    <t xml:space="preserve">Black-Billed Magpie</t>
   </si>
   <si>
     <t xml:space="preserve">Pica hudsonia</t>
@@ -523,7 +523,7 @@
     <t xml:space="preserve">Wszyscy gracze otrzymują po 1 [fruit] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black-Crowned Night-Heron </t>
+    <t xml:space="preserve">Black-Crowned Night-Heron</t>
   </si>
   <si>
     <t xml:space="preserve">Nycticorax nycticorax</t>
@@ -547,7 +547,7 @@
     <t xml:space="preserve">Pożywienie, które ten gracz bierze z karmnika, nie musi być tego samego rodzaju co pożywienie zabrane przez Ciebie z jego zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black-Necked Stilt </t>
+    <t xml:space="preserve">Black-Necked Stilt</t>
   </si>
   <si>
     <t xml:space="preserve">Himantopus mexicanus</t>
@@ -607,7 +607,7 @@
     <t xml:space="preserve">Modrosójka Błękitna</t>
   </si>
   <si>
-    <t xml:space="preserve">Blue-Gray Gnatcatcher </t>
+    <t xml:space="preserve">Blue-Gray Gnatcatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Polioptila caerulea</t>
@@ -679,7 +679,7 @@
     <t xml:space="preserve">Dobierz 3 odkryte [card] z tacki.</t>
   </si>
   <si>
-    <t xml:space="preserve">Brewer's Blackbird </t>
+    <t xml:space="preserve">Brewer's Blackbird</t>
   </si>
   <si>
     <t xml:space="preserve">Euphagus cyanocephalus</t>
@@ -700,7 +700,7 @@
     <t xml:space="preserve">Myszołów Szerokoskrzydły</t>
   </si>
   <si>
-    <t xml:space="preserve">Bronzed Cowbird </t>
+    <t xml:space="preserve">Bronzed Cowbird</t>
   </si>
   <si>
     <t xml:space="preserve">Molothrus aeneus</t>
@@ -724,7 +724,7 @@
     <t xml:space="preserve">Weź 3 [fish] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Brown-Headed Cowbird </t>
+    <t xml:space="preserve">Brown-Headed Cowbird</t>
   </si>
   <si>
     <t xml:space="preserve">Molothrus ater</t>
@@ -748,7 +748,7 @@
     <t xml:space="preserve">Jeśli po napełnieniu karmnika nie ma w nim określonego rodzaju pożywienia, nie otrzymujesz pożywienia.</t>
   </si>
   <si>
-    <t xml:space="preserve">Burrowing Owl </t>
+    <t xml:space="preserve">Burrowing Owl</t>
   </si>
   <si>
     <t xml:space="preserve">Athene cunicularia</t>
@@ -775,7 +775,7 @@
     <t xml:space="preserve">Kondor Kalifornijski</t>
   </si>
   <si>
-    <t xml:space="preserve">California Quail </t>
+    <t xml:space="preserve">California Quail</t>
   </si>
   <si>
     <t xml:space="preserve">Callipepla californica</t>
@@ -787,7 +787,7 @@
     <t xml:space="preserve">Złóż 1 [egg] i połóż na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Canada Goose </t>
+    <t xml:space="preserve">Canada Goose</t>
   </si>
   <si>
     <t xml:space="preserve">Branta canadensis</t>
@@ -808,7 +808,7 @@
     <t xml:space="preserve">Wszyscy gracze dobierają 1 [card] ze stosu.</t>
   </si>
   <si>
-    <t xml:space="preserve">Carolina Chickadee </t>
+    <t xml:space="preserve">Carolina Chickadee</t>
   </si>
   <si>
     <t xml:space="preserve">Poecile carolinensis</t>
@@ -850,7 +850,7 @@
     <t xml:space="preserve">Dziwuszka Czerwonoczelna</t>
   </si>
   <si>
-    <t xml:space="preserve">Cassin's Sparrow </t>
+    <t xml:space="preserve">Cassin's Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Peucaea cassinii</t>
@@ -871,7 +871,7 @@
     <t xml:space="preserve">Wsuń [card] z ręki pod tę kartę. Jeśli to zrobisz, weź 1 [fruit] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cerulean Warbler </t>
+    <t xml:space="preserve">Cerulean Warbler</t>
   </si>
   <si>
     <t xml:space="preserve">Setophaga cerulea</t>
@@ -895,7 +895,7 @@
     <t xml:space="preserve">Te ptaki liczą się podwójnie tylko na potrzeby realizacji celów, ale już nie w przypadku kart bonusowych czy punktów na koniec gry.&lt;br&gt;Jaja na kartach tych ptaków nie liczą się podwójnie na potrzeby realizacji celów zliczających jaja.</t>
   </si>
   <si>
-    <t xml:space="preserve">Chestnut-Collared Longspur </t>
+    <t xml:space="preserve">Chestnut-Collared Longspur</t>
   </si>
   <si>
     <t xml:space="preserve">Calcarius ornatus</t>
@@ -925,7 +925,7 @@
     <t xml:space="preserve">Kominiarczyk Amerykański</t>
   </si>
   <si>
-    <t xml:space="preserve">Chipping Sparrow </t>
+    <t xml:space="preserve">Chipping Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Spizella passerina</t>
@@ -934,7 +934,7 @@
     <t xml:space="preserve">Spizela Białobrewa</t>
   </si>
   <si>
-    <t xml:space="preserve">Clark's Grebe </t>
+    <t xml:space="preserve">Clark's Grebe</t>
   </si>
   <si>
     <t xml:space="preserve">Aechmophorus clarkii</t>
@@ -943,7 +943,7 @@
     <t xml:space="preserve">Perkoz Żółtodzioby</t>
   </si>
   <si>
-    <t xml:space="preserve">Clark's Nutcracker </t>
+    <t xml:space="preserve">Clark's Nutcracker</t>
   </si>
   <si>
     <t xml:space="preserve">Nucifraga columbiana</t>
@@ -1051,7 +1051,7 @@
     <t xml:space="preserve">W przypadku zdolności tego ptaka symbol [star] liczy się jako [cavity].</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Grackle </t>
+    <t xml:space="preserve">Common Grackle</t>
   </si>
   <si>
     <t xml:space="preserve">Quiscalus quiscula</t>
@@ -1096,7 +1096,7 @@
     <t xml:space="preserve">Nur Lodowiec</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Merganser </t>
+    <t xml:space="preserve">Common Merganser</t>
   </si>
   <si>
     <t xml:space="preserve">Mergus merganser</t>
@@ -1120,7 +1120,7 @@
     <t xml:space="preserve">Jeśli zagrany ptak ma zdolność „GDY ZAGRYWASZ”, aktywuje się ona w momencie zagrania.</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Nighthawk </t>
+    <t xml:space="preserve">Common Nighthawk</t>
   </si>
   <si>
     <t xml:space="preserve">Chordeiles minor</t>
@@ -1171,7 +1171,7 @@
     <t xml:space="preserve">Odrzuć do 5 [invertebrate] ze swoich zasobów. Za każdy odrzucony żeton wsuń po 1 [card] ze stosu pod tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Yellowthroat </t>
+    <t xml:space="preserve">Common Yellowthroat</t>
   </si>
   <si>
     <t xml:space="preserve">Geothlypis trichas</t>
@@ -1183,7 +1183,7 @@
     <t xml:space="preserve">Dobierz 2 [card]. Jeśli to zrobisz, na koniec tury odrzuć 1 [card] z ręki.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cooper's Hawk </t>
+    <t xml:space="preserve">Cooper's Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Accipiter cooperii</t>
@@ -1225,7 +1225,7 @@
     <t xml:space="preserve">Łuszczyk Czarnogardły</t>
   </si>
   <si>
-    <t xml:space="preserve">Double-Crested Cormorant </t>
+    <t xml:space="preserve">Double-Crested Cormorant</t>
   </si>
   <si>
     <t xml:space="preserve">Phalacrocorax auritus</t>
@@ -1234,7 +1234,7 @@
     <t xml:space="preserve">Kormoran Rogaty</t>
   </si>
   <si>
-    <t xml:space="preserve">Downy Woodpecker </t>
+    <t xml:space="preserve">Downy Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Picoides pubescens</t>
@@ -1294,7 +1294,7 @@
     <t xml:space="preserve">Gdy inny gracz zagrywa ptaka na [forest], weź 1 [invertebrate] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Eastern Phoebe </t>
+    <t xml:space="preserve">Eastern Phoebe</t>
   </si>
   <si>
     <t xml:space="preserve">Sayornis phoebe</t>
@@ -1306,7 +1306,7 @@
     <t xml:space="preserve">Wszyscy gracze otrzymują 1 [invertebrate] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Eastern Screech Owl </t>
+    <t xml:space="preserve">Eastern Screech Owl</t>
   </si>
   <si>
     <t xml:space="preserve">Megascops asio</t>
@@ -1516,7 +1516,7 @@
     <t xml:space="preserve">Dobierz 1 nową kartę bonusową. Następnie weź 1 [die] z karmnika, złóż 1 [egg] na karcie dowolnego ptaka albo dobierz 1 [card].</t>
   </si>
   <si>
-    <t xml:space="preserve">Ferruginous Hawk </t>
+    <t xml:space="preserve">Ferruginous Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Buteo regalis</t>
@@ -1534,7 +1534,7 @@
     <t xml:space="preserve">Wrona Rybożerna</t>
   </si>
   <si>
-    <t xml:space="preserve">Forster's Tern </t>
+    <t xml:space="preserve">Forster's Tern</t>
   </si>
   <si>
     <t xml:space="preserve">Sterna forsteri</t>
@@ -1543,7 +1543,7 @@
     <t xml:space="preserve">Rybitwa Czarnoucha</t>
   </si>
   <si>
-    <t xml:space="preserve">Franklin's Gull </t>
+    <t xml:space="preserve">Franklin's Gull</t>
   </si>
   <si>
     <t xml:space="preserve">Leucophaeus pipixcan</t>
@@ -1582,7 +1582,7 @@
     <t xml:space="preserve">Podejrzyj [card] ze stosu. Jeśli &lt;100 cm, wsuń kartę ofiary pod tę kartę. Jeśli nie spełnia warunku, odrzuć.</t>
   </si>
   <si>
-    <t xml:space="preserve">Grasshopper Sparrow </t>
+    <t xml:space="preserve">Grasshopper Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Ammodramus savannarum</t>
@@ -1618,7 +1618,7 @@
     <t xml:space="preserve">Zagraj drugiego ptaka na [wetland]. Zapłać jego standardowy koszt.</t>
   </si>
   <si>
-    <t xml:space="preserve">Great Crested Flycatcher </t>
+    <t xml:space="preserve">Great Crested Flycatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Myiarchus crinitus</t>
@@ -1654,7 +1654,7 @@
     <t xml:space="preserve">Czapla Biała</t>
   </si>
   <si>
-    <t xml:space="preserve">Great Horned Owl </t>
+    <t xml:space="preserve">Great Horned Owl</t>
   </si>
   <si>
     <t xml:space="preserve">Bubo virginianus</t>
@@ -1690,7 +1690,7 @@
     <t xml:space="preserve">Możesz wsunąć maksymalnie tyle kart, ile wynosi liczba kostek akcji wybranego gracza w danym siedlisku.</t>
   </si>
   <si>
-    <t xml:space="preserve">Greater Prairie Chicken </t>
+    <t xml:space="preserve">Greater Prairie Chicken</t>
   </si>
   <si>
     <t xml:space="preserve">Tympanuchus cupido</t>
@@ -1699,7 +1699,7 @@
     <t xml:space="preserve">Preriokur Dwuczuby</t>
   </si>
   <si>
-    <t xml:space="preserve">Greater Roadrunner </t>
+    <t xml:space="preserve">Greater Roadrunner</t>
   </si>
   <si>
     <t xml:space="preserve">Geococcyx californianus</t>
@@ -1870,7 +1870,7 @@
     <t xml:space="preserve">Połóż 1 [egg] na każdej swojej karcie ptaka z gniazdem [platform].</t>
   </si>
   <si>
-    <t xml:space="preserve">Indigo Bunting </t>
+    <t xml:space="preserve">Indigo Bunting</t>
   </si>
   <si>
     <t xml:space="preserve">Passerina cyanea</t>
@@ -1882,7 +1882,7 @@
     <t xml:space="preserve">Weź 1 [invertebrate] albo [fruit] z karmnika (jeśli są dostępne).</t>
   </si>
   <si>
-    <t xml:space="preserve">Juniper Titmouse </t>
+    <t xml:space="preserve">Juniper Titmouse</t>
   </si>
   <si>
     <t xml:space="preserve">Baeolophus ridgwayi</t>
@@ -1909,7 +1909,7 @@
     <t xml:space="preserve">Wodnik Królewski</t>
   </si>
   <si>
-    <t xml:space="preserve">Lazuli Bunting </t>
+    <t xml:space="preserve">Lazuli Bunting</t>
   </si>
   <si>
     <t xml:space="preserve">Passerina amoena</t>
@@ -2032,7 +2032,7 @@
     <t xml:space="preserve">Błotniak Łąkowy</t>
   </si>
   <si>
-    <t xml:space="preserve">Mountain Bluebird </t>
+    <t xml:space="preserve">Mountain Bluebird</t>
   </si>
   <si>
     <t xml:space="preserve">Sialia currucoides</t>
@@ -2041,7 +2041,7 @@
     <t xml:space="preserve">Błękitnik Górski</t>
   </si>
   <si>
-    <t xml:space="preserve">Mountain Chickadee </t>
+    <t xml:space="preserve">Mountain Chickadee</t>
   </si>
   <si>
     <t xml:space="preserve">Poecile gambeli</t>
@@ -2050,7 +2050,7 @@
     <t xml:space="preserve">Sikora Górska</t>
   </si>
   <si>
-    <t xml:space="preserve">Mourning Dove </t>
+    <t xml:space="preserve">Mourning Dove</t>
   </si>
   <si>
     <t xml:space="preserve">Zenaida macroura</t>
@@ -2083,7 +2083,7 @@
     <t xml:space="preserve">Przepiór Wirginijski</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Cardinal </t>
+    <t xml:space="preserve">Northern Cardinal</t>
   </si>
   <si>
     <t xml:space="preserve">Cardinalis cardinalis</t>
@@ -2125,7 +2125,7 @@
     <t xml:space="preserve">Jastrząb Zwyczajny</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Harrier </t>
+    <t xml:space="preserve">Northern Harrier</t>
   </si>
   <si>
     <t xml:space="preserve">Circus cyaneus</t>
@@ -2134,7 +2134,7 @@
     <t xml:space="preserve">Błotniak Zbożowy</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Mockingbird </t>
+    <t xml:space="preserve">Northern Mockingbird</t>
   </si>
   <si>
     <t xml:space="preserve">Mimus polyglottos</t>
@@ -2143,7 +2143,7 @@
     <t xml:space="preserve">Przedrzeźniacz Północny</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Shoveler </t>
+    <t xml:space="preserve">Northern Shoveler</t>
   </si>
   <si>
     <t xml:space="preserve">Spatula clypeata</t>
@@ -2167,7 +2167,7 @@
     <t xml:space="preserve">Wszyscy gracze otrzymują 1 [fish] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Painted Bunting </t>
+    <t xml:space="preserve">Painted Bunting</t>
   </si>
   <si>
     <t xml:space="preserve">Passerina ciris</t>
@@ -2200,7 +2200,7 @@
     <t xml:space="preserve">Otrzymujesz [seed] bez względu na to, jaką kość pożywienia usunąłeś z karmnika.</t>
   </si>
   <si>
-    <t xml:space="preserve">Peregrine Falcon </t>
+    <t xml:space="preserve">Peregrine Falcon</t>
   </si>
   <si>
     <t xml:space="preserve">Falco peregrinus</t>
@@ -2209,7 +2209,7 @@
     <t xml:space="preserve">Sokół Wędrowny</t>
   </si>
   <si>
-    <t xml:space="preserve">Pied-Billed Grebe </t>
+    <t xml:space="preserve">Pied-Billed Grebe</t>
   </si>
   <si>
     <t xml:space="preserve">Podilymbus podiceps</t>
@@ -2218,7 +2218,7 @@
     <t xml:space="preserve">Perkoz Grubodzioby</t>
   </si>
   <si>
-    <t xml:space="preserve">Pileated Woodpecker </t>
+    <t xml:space="preserve">Pileated Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Dryocopus pileatus</t>
@@ -2248,7 +2248,7 @@
     <t xml:space="preserve">Bursztynka</t>
   </si>
   <si>
-    <t xml:space="preserve">Purple Gallinule </t>
+    <t xml:space="preserve">Purple Gallinule</t>
   </si>
   <si>
     <t xml:space="preserve">Porphyrio martinicus</t>
@@ -2320,7 +2320,7 @@
     <t xml:space="preserve">Zabierz 1 [invertebrate] z zasobów innego gracza i przechowaj na tej karcie. Ten gracz bierze 1 [die] z karmnika.</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Bellied Woodpecker </t>
+    <t xml:space="preserve">Red-Bellied Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Melanerpes carolinus</t>
@@ -2338,7 +2338,7 @@
     <t xml:space="preserve">Szlachar</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Breasted Nuthatch </t>
+    <t xml:space="preserve">Red-Breasted Nuthatch</t>
   </si>
   <si>
     <t xml:space="preserve">Sitta canadensis</t>
@@ -2347,7 +2347,7 @@
     <t xml:space="preserve">Kowalik Czarnogłowy</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Cockaded Woodpecker </t>
+    <t xml:space="preserve">Red-Cockaded Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Picoides borealis</t>
@@ -2356,7 +2356,7 @@
     <t xml:space="preserve">Dzięcioł Skromny</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Eyed Vireo </t>
+    <t xml:space="preserve">Red-Eyed Vireo</t>
   </si>
   <si>
     <t xml:space="preserve">Vireo olivaceus</t>
@@ -2365,7 +2365,7 @@
     <t xml:space="preserve">Wireonek Czerwonooki</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Headed Woodpecker </t>
+    <t xml:space="preserve">Red-Headed Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Melanerpes erythrocephalus</t>
@@ -2386,7 +2386,7 @@
     <t xml:space="preserve">Złóż 1 [egg] na każdej karcie ptaka w tej kolumnie, włączając tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Shouldered Hawk </t>
+    <t xml:space="preserve">Red-Shouldered Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Buteo lineatus</t>
@@ -2395,7 +2395,7 @@
     <t xml:space="preserve">Myszołów Rdzawoskrzydły</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Tailed Hawk </t>
+    <t xml:space="preserve">Red-Tailed Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Buteo jamaicensis</t>
@@ -2404,7 +2404,7 @@
     <t xml:space="preserve">Myszołów Rdzawosterny</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Winged Blackbird </t>
+    <t xml:space="preserve">Red-Winged Blackbird</t>
   </si>
   <si>
     <t xml:space="preserve">Agelaius phoeniceus</t>
@@ -2422,7 +2422,7 @@
     <t xml:space="preserve">Mewa Delawarska</t>
   </si>
   <si>
-    <t xml:space="preserve">Rose-Breasted Grosbeak </t>
+    <t xml:space="preserve">Rose-Breasted Grosbeak</t>
   </si>
   <si>
     <t xml:space="preserve">Pheucticus ludovicianus</t>
@@ -2434,7 +2434,7 @@
     <t xml:space="preserve">Weź 1 [seed] albo [fruit] z karmnika (jeśli są dostępne).</t>
   </si>
   <si>
-    <t xml:space="preserve">Roseate Spoonbill </t>
+    <t xml:space="preserve">Roseate Spoonbill</t>
   </si>
   <si>
     <t xml:space="preserve">Platalea ajaja</t>
@@ -2443,7 +2443,7 @@
     <t xml:space="preserve">Warzęcha Różowa</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruby-Crowned Kinglet </t>
+    <t xml:space="preserve">Ruby-Crowned Kinglet</t>
   </si>
   <si>
     <t xml:space="preserve">Regulus calendula</t>
@@ -2491,7 +2491,7 @@
     <t xml:space="preserve">Żuraw Kanadyjski</t>
   </si>
   <si>
-    <t xml:space="preserve">Savannah Sparrow </t>
+    <t xml:space="preserve">Savannah Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Passerculus sandwichensis</t>
@@ -2539,7 +2539,7 @@
     <t xml:space="preserve">Złóż 1 [egg] na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Scissor-Tailed Flycatcher </t>
+    <t xml:space="preserve">Scissor-Tailed Flycatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Tyrannus forficatus</t>
@@ -2572,7 +2572,7 @@
     <t xml:space="preserve">Gdy inny gracz z jakiegokolwiek powodu wsuwa [card], wsuń 1 [card] z ręki pod tę kartę. Następnie dobierz 1 [card] na koniec jego tury.</t>
   </si>
   <si>
-    <t xml:space="preserve">Snowy Egret </t>
+    <t xml:space="preserve">Snowy Egret</t>
   </si>
   <si>
     <t xml:space="preserve">Egretta thula</t>
@@ -2590,7 +2590,7 @@
     <t xml:space="preserve">Puchacz Śnieżny</t>
   </si>
   <si>
-    <t xml:space="preserve">Song Sparrow </t>
+    <t xml:space="preserve">Song Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Melospiza melodia</t>
@@ -2608,7 +2608,7 @@
     <t xml:space="preserve">Puszczyk Plamisty</t>
   </si>
   <si>
-    <t xml:space="preserve">Spotted Sandpiper </t>
+    <t xml:space="preserve">Spotted Sandpiper</t>
   </si>
   <si>
     <t xml:space="preserve">Actitis macularius</t>
@@ -2617,7 +2617,7 @@
     <t xml:space="preserve">Brodziec Plamisty</t>
   </si>
   <si>
-    <t xml:space="preserve">Spotted Towhee </t>
+    <t xml:space="preserve">Spotted Towhee</t>
   </si>
   <si>
     <t xml:space="preserve">Pipilo maculatus</t>
@@ -2680,7 +2680,7 @@
     <t xml:space="preserve">Odrzuć 1 [seed] ze swoich zasobów. Jeśli to zrobisz, złóż 2 [egg] na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Tree Swallow </t>
+    <t xml:space="preserve">Tree Swallow</t>
   </si>
   <si>
     <t xml:space="preserve">Tachycineta bicolor</t>
@@ -2728,7 +2728,7 @@
     <t xml:space="preserve">Wsuń [card] z ręki pod tę kartę. Jeśli to zrobisz, weź 1 [invertebrate] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Violet-Green Swallow </t>
+    <t xml:space="preserve">Violet-Green Swallow</t>
   </si>
   <si>
     <t xml:space="preserve">Tachycineta thalassina</t>
@@ -2791,7 +2791,7 @@
     <t xml:space="preserve">Jeśli wszystkie kości w karmniku wskazują ten sam symbol, możesz go opróżnić i ponownie napełnić przed pobraniem [die].</t>
   </si>
   <si>
-    <t xml:space="preserve">White-Breasted Nuthatch </t>
+    <t xml:space="preserve">White-Breasted Nuthatch</t>
   </si>
   <si>
     <t xml:space="preserve">Sitta carolinensis</t>
@@ -2800,7 +2800,7 @@
     <t xml:space="preserve">Kowalik Karoliński</t>
   </si>
   <si>
-    <t xml:space="preserve">White-Crowned Sparrow </t>
+    <t xml:space="preserve">White-Crowned Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Zonotrichia leucophrys</t>
@@ -2809,7 +2809,7 @@
     <t xml:space="preserve">Pasówka Białobrewa</t>
   </si>
   <si>
-    <t xml:space="preserve">White-Faced Ibis </t>
+    <t xml:space="preserve">White-Faced Ibis</t>
   </si>
   <si>
     <t xml:space="preserve">Plegadis chihi</t>
@@ -2902,7 +2902,7 @@
     <t xml:space="preserve">Dławigad Amerykański</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Bellied Sapsucker </t>
+    <t xml:space="preserve">Yellow-Bellied Sapsucker</t>
   </si>
   <si>
     <t xml:space="preserve">Sphyrapicus varius</t>
@@ -2920,7 +2920,7 @@
     <t xml:space="preserve">Kukawik Żółtodzioby</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Breasted Chat </t>
+    <t xml:space="preserve">Yellow-Breasted Chat</t>
   </si>
   <si>
     <t xml:space="preserve">Icteria virens</t>
@@ -2929,7 +2929,7 @@
     <t xml:space="preserve">Słowikówka</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Headed Blackbird </t>
+    <t xml:space="preserve">Yellow-Headed Blackbird</t>
   </si>
   <si>
     <t xml:space="preserve">Xanthocephalus xanthocephalus</t>
@@ -2938,7 +2938,7 @@
     <t xml:space="preserve">Żółtogłowiec</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Rumped Warbler </t>
+    <t xml:space="preserve">Yellow-Rumped Warbler</t>
   </si>
   <si>
     <t xml:space="preserve">Setophaga coronata</t>
@@ -6031,30 +6031,6 @@
     <t xml:space="preserve">Szereg ptaków w [wetland] o rosnącej albo malejącej rozpiętości skrzydeł.</t>
   </si>
   <si>
-    <t xml:space="preserve">[automa] Avid Asian Avian Admirer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[automa] Zagorzały miłośnik ptaków azjatyckich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;2&lt;/b&gt; albo &lt;b&gt;3&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;3&lt;/b&gt; albo &lt;b&gt;4&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt; albo &lt;b&gt;5&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Zaczyna od kart z niższą wartością).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[automa] Rare Species Lister</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[automa] Znawca rzadkich gatunków</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt;, &lt;b&gt;5&lt;/b&gt; albo &lt;b&gt;6&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;5&lt;/b&gt;, &lt;b&gt;6&lt;/b&gt; albo &lt;b&gt;7&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;6&lt;/b&gt;, &lt;b&gt;7&lt;/b&gt; albo &lt;b&gt;8&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automa zatrzymuje kartę o najniższej wartości.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Avian Theriogenologist</t>
   </si>
   <si>
@@ -6273,6 +6249,30 @@
   </si>
   <si>
     <t xml:space="preserve">Policz, ile niewykorzystanych żetonów pożywienia masz na koniec gry w swoich zasobach. Pożywienie przechowywane na kartach ptaków nie liczy się jako część zasobów.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Avid Asian Avian Admirer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Zagorzały miłośnik ptaków azjatyckich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;2&lt;/b&gt; albo &lt;b&gt;3&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;3&lt;/b&gt; albo &lt;b&gt;4&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt; albo &lt;b&gt;5&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Zaczyna od kart z niższą wartością).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Rare Species Lister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Znawca rzadkich gatunków</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt;, &lt;b&gt;5&lt;/b&gt; albo &lt;b&gt;6&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;5&lt;/b&gt;, &lt;b&gt;6&lt;/b&gt; albo &lt;b&gt;7&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;6&lt;/b&gt;, &lt;b&gt;7&lt;/b&gt; albo &lt;b&gt;8&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automa zatrzymuje kartę o najniższej wartości.</t>
   </si>
   <si>
     <t xml:space="preserve">Translated</t>
@@ -6507,7 +6507,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6515,7 +6515,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6568,6 +6568,112 @@
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -6575,8 +6681,10 @@
   </sheetPr>
   <dimension ref="A1:K447"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="C271" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G271" activeCellId="0" sqref="G271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18824,7 +18932,7 @@
       <c r="J433" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K433" s="0" t="s">
+      <c r="K433" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -19255,8 +19363,10 @@
   </sheetPr>
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19265,7 +19375,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="53.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.88"/>
@@ -20227,7 +20337,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
-        <v>1050</v>
+        <v>1039</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>1956</v>
@@ -20235,166 +20345,169 @@
       <c r="C40" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="1" t="s">
         <v>1957</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="1" t="s">
         <v>1958</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="1" t="s">
         <v>1959</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>1928</v>
+      <c r="G40" s="9" t="s">
+        <v>1960</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>1961</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
-        <v>1051</v>
+        <v>1040</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>1960</v>
+        <v>1962</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>1961</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>1962</v>
-      </c>
-      <c r="G41" s="4" t="s">
+      <c r="D41" s="1" t="s">
         <v>1963</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>1964</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>1965</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>1966</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>1964</v>
+        <v>1967</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1965</v>
+        <v>1968</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1966</v>
+        <v>1969</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1967</v>
+        <v>1970</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>1968</v>
+        <v>1971</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>1969</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>1970</v>
+        <v>1973</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1971</v>
+        <v>1974</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1972</v>
+        <v>1975</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>1973</v>
+        <v>1936</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>1974</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="n">
-        <v>1041</v>
+      <c r="A44" s="9" t="n">
+        <v>1043</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>1975</v>
+        <v>1977</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>1976</v>
+        <v>1978</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1977</v>
+        <v>1979</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1978</v>
+        <v>1970</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>1979</v>
+        <v>1971</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>1980</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>1982</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>1983</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>1936</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>1984</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="n">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>1984</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>1985</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>1986</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>1987</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>1978</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>1979</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>1980</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>1988</v>
@@ -20408,39 +20521,45 @@
       <c r="E47" s="1" t="s">
         <v>1990</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>1991</v>
+      </c>
       <c r="G47" s="9" t="s">
-        <v>1936</v>
+        <v>1818</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>1984</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="n">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>1991</v>
+        <v>1993</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1992</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>1993</v>
+        <v>1994</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>1995</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>1970</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>1994</v>
+        <v>1971</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>1995</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>1996</v>
@@ -20454,45 +20573,39 @@
       <c r="E49" s="1" t="s">
         <v>1998</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>1999</v>
-      </c>
       <c r="G49" s="9" t="s">
-        <v>1818</v>
+        <v>1936</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>2000</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="n">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>2000</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>2002</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>2003</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>1978</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>1979</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>1980</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>2004</v>
@@ -20500,39 +20613,36 @@
       <c r="C51" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="9" t="s">
         <v>2005</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="9" t="s">
         <v>2006</v>
       </c>
-      <c r="G51" s="9" t="s">
-        <v>1936</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>1984</v>
+      <c r="F51" s="4" t="s">
+        <v>2007</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>1928</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="n">
-        <v>1049</v>
+      <c r="A52" s="2" t="n">
+        <v>1051</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>2008</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="D52" s="9" t="s">
         <v>2009</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="E52" s="9" t="s">
         <v>2010</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="G52" s="4" t="s">
         <v>2011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
translations fixes, new data (#54)
</commit_message>
<xml_diff>
--- a/i18n/pl.xlsx
+++ b/i18n/pl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Birds" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Other" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Birds" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Bonuses" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Other" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="ExternalData_1" vbProcedure="false">Birds!$A$1:$G$357</definedName>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">Ptaki obdarzone tą zdolnością znane są z przechowywania pożywienia na później. Zdolność ta pozwala przechować (położyć na karcie ptaka) 1 żeton pożywienia podczas każdej aktywacji tej karty. Przechowywane na karcie żetony nie mogą zostać wykorzystane w trakcie gry. Każdy z tych żetonów jest wart 1 punkt na koniec gry.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Avocet </t>
+    <t xml:space="preserve">American Avocet</t>
   </si>
   <si>
     <t xml:space="preserve">Recurvirostra americana</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">X</t>
   </si>
   <si>
-    <t xml:space="preserve">American Bittern </t>
+    <t xml:space="preserve">American Bittern</t>
   </si>
   <si>
     <t xml:space="preserve">Botaurus lentiginosus</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Pod karty tych ptaków możesz wsunąć kartę z ręki. Na koniec gry za każdą wsuniętą kartę otrzymasz 1 punkt. Dodatkowo karty ptaków z tej grupy oferują jeszcze jakąś korzyść (złożenie jaja, dobranie karty, zdobycie pożywienia). Możesz z niej skorzystać tylko wtedy, gdy najpierw wsunąłeś kartę z ręki pod tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Crow </t>
+    <t xml:space="preserve">American Crow</t>
   </si>
   <si>
     <t xml:space="preserve">Corvus brachyrhynchos</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">Te gatunki znane są z podjadania jaj z gniazd innych ptaków. Aby użyć tej zdolności, musisz mieć już złożone wcześniej jajo na innym ptaku. Odrzuć jajo do zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Goldfinch </t>
+    <t xml:space="preserve">American Goldfinch</t>
   </si>
   <si>
     <t xml:space="preserve">Spinus tristis</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Weź 3 [seed] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">American Kestrel </t>
+    <t xml:space="preserve">American Kestrel</t>
   </si>
   <si>
     <t xml:space="preserve">Falco sparverius</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">Drozd Wędrowny</t>
   </si>
   <si>
-    <t xml:space="preserve">American White Pelican </t>
+    <t xml:space="preserve">American White Pelican</t>
   </si>
   <si>
     <t xml:space="preserve">Pelecanus erythrorhynchos</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">Rzuć wszystkimi kośćmi znajdującymi się poza karmnikiem. Jeśli choć 1 kość wskaże [fish], weź 1 [fish] i przechowaj na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Anna's Hummingbird </t>
+    <t xml:space="preserve">Anna's Hummingbird</t>
   </si>
   <si>
     <t xml:space="preserve">Calypte anna</t>
@@ -259,7 +259,7 @@
     <t xml:space="preserve">Właściciel kolibra decyduje, kto otrzymuje pożywienie jako pierwszy, a następnie obowiązuje kolejność rozgrywania. Gracze mogą napełniać karmnik, gdy opustoszeje, a także gdy wszystkie kości wskazują ten sam symbol (dotyczy także pojedynczej kostki).</t>
   </si>
   <si>
-    <t xml:space="preserve">Ash-Throated Flycatcher </t>
+    <t xml:space="preserve">Ash-Throated Flycatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Myiarchus cinerascens</t>
@@ -304,7 +304,7 @@
     <t xml:space="preserve">Dobierz 2 [card] ze stosu. Wsuń 1 z nich pod tę kartę i zatrzymaj drugą.</t>
   </si>
   <si>
-    <t xml:space="preserve">Baird's Sparrow </t>
+    <t xml:space="preserve">Baird's Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Ammodramus bairdii</t>
@@ -316,7 +316,7 @@
     <t xml:space="preserve">Złóż 1 [egg] i połóż na swojej dowolnej karcie ptaka.</t>
   </si>
   <si>
-    <t xml:space="preserve">Bald Eagle </t>
+    <t xml:space="preserve">Bald Eagle</t>
   </si>
   <si>
     <t xml:space="preserve">Haliaeetus leucocephalus</t>
@@ -328,7 +328,7 @@
     <t xml:space="preserve">Weź wszystkie [fish] z karmnika.</t>
   </si>
   <si>
-    <t xml:space="preserve">Baltimore Oriole </t>
+    <t xml:space="preserve">Baltimore Oriole</t>
   </si>
   <si>
     <t xml:space="preserve">Icterus galbula</t>
@@ -373,7 +373,7 @@
     <t xml:space="preserve">Te ptaki żywią się innymi ptakami. Porównaj rozpiętość skrzydeł wierzchniej karty ze stosu ze zdolnością drapieżnika.&lt;br&gt;Jeśli rozpiętość skrzydeł na wierzchniej karcie ze stosu jest mniejsza od limitu zdolności drapieżnika, wsuń tę kartę pod swoją kartę, aby zaznaczyć, że Twój drapieżnik skutecznie zapolował. Na koniec gry każda taka wsunięta karta warta jest 1 punkt.&lt;br&gt;Jeśli rozpiętość skrzydeł wierzchniej karty jest równa lub większa od zdolności Twojego drapieżnika, odrzuć ją.</t>
   </si>
   <si>
-    <t xml:space="preserve">Barrow's Goldeneye </t>
+    <t xml:space="preserve">Barrow's Goldeneye</t>
   </si>
   <si>
     <t xml:space="preserve">Bucephala islandica</t>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">Wireonek Skromny</t>
   </si>
   <si>
-    <t xml:space="preserve">Belted Kingfisher </t>
+    <t xml:space="preserve">Belted Kingfisher</t>
   </si>
   <si>
     <t xml:space="preserve">Megaceryle alcyon</t>
@@ -436,7 +436,7 @@
     <t xml:space="preserve">Wybierz siedlisko bez żadnych [egg]. Złóż 1 [egg] na każdej karcie w tym siedlisku.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black Skimmer </t>
+    <t xml:space="preserve">Black Skimmer</t>
   </si>
   <si>
     <t xml:space="preserve">Rynchops niger</t>
@@ -460,7 +460,7 @@
     <t xml:space="preserve">Ta zdolność pozwala dobrać dodatkowe karty ptaków podczas wykonywania akcji „Dobierz karty ptaków”, ale ma swój koszt (odrzucenie karty). Gdy zastanawiasz się, którą kartę odrzucić, kolejny gracz może zacząć swoją turę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black Vulture </t>
+    <t xml:space="preserve">Black Vulture</t>
   </si>
   <si>
     <t xml:space="preserve">Coragyps atratus</t>
@@ -502,7 +502,7 @@
     <t xml:space="preserve">Odrzuć 1 [seed], aby wsunąć 2 [card] ze stosu pod tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black-Billed Magpie </t>
+    <t xml:space="preserve">Black-Billed Magpie</t>
   </si>
   <si>
     <t xml:space="preserve">Pica hudsonia</t>
@@ -523,7 +523,7 @@
     <t xml:space="preserve">Wszyscy gracze otrzymują po 1 [fruit] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black-Crowned Night-Heron </t>
+    <t xml:space="preserve">Black-Crowned Night-Heron</t>
   </si>
   <si>
     <t xml:space="preserve">Nycticorax nycticorax</t>
@@ -547,7 +547,7 @@
     <t xml:space="preserve">Pożywienie, które ten gracz bierze z karmnika, nie musi być tego samego rodzaju co pożywienie zabrane przez Ciebie z jego zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Black-Necked Stilt </t>
+    <t xml:space="preserve">Black-Necked Stilt</t>
   </si>
   <si>
     <t xml:space="preserve">Himantopus mexicanus</t>
@@ -607,7 +607,7 @@
     <t xml:space="preserve">Modrosójka Błękitna</t>
   </si>
   <si>
-    <t xml:space="preserve">Blue-Gray Gnatcatcher </t>
+    <t xml:space="preserve">Blue-Gray Gnatcatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Polioptila caerulea</t>
@@ -679,7 +679,7 @@
     <t xml:space="preserve">Dobierz 3 odkryte [card] z tacki.</t>
   </si>
   <si>
-    <t xml:space="preserve">Brewer's Blackbird </t>
+    <t xml:space="preserve">Brewer's Blackbird</t>
   </si>
   <si>
     <t xml:space="preserve">Euphagus cyanocephalus</t>
@@ -700,7 +700,7 @@
     <t xml:space="preserve">Myszołów Szerokoskrzydły</t>
   </si>
   <si>
-    <t xml:space="preserve">Bronzed Cowbird </t>
+    <t xml:space="preserve">Bronzed Cowbird</t>
   </si>
   <si>
     <t xml:space="preserve">Molothrus aeneus</t>
@@ -724,7 +724,7 @@
     <t xml:space="preserve">Weź 3 [fish] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Brown-Headed Cowbird </t>
+    <t xml:space="preserve">Brown-Headed Cowbird</t>
   </si>
   <si>
     <t xml:space="preserve">Molothrus ater</t>
@@ -748,7 +748,7 @@
     <t xml:space="preserve">Jeśli po napełnieniu karmnika nie ma w nim określonego rodzaju pożywienia, nie otrzymujesz pożywienia.</t>
   </si>
   <si>
-    <t xml:space="preserve">Burrowing Owl </t>
+    <t xml:space="preserve">Burrowing Owl</t>
   </si>
   <si>
     <t xml:space="preserve">Athene cunicularia</t>
@@ -775,7 +775,7 @@
     <t xml:space="preserve">Kondor Kalifornijski</t>
   </si>
   <si>
-    <t xml:space="preserve">California Quail </t>
+    <t xml:space="preserve">California Quail</t>
   </si>
   <si>
     <t xml:space="preserve">Callipepla californica</t>
@@ -787,7 +787,7 @@
     <t xml:space="preserve">Złóż 1 [egg] i połóż na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Canada Goose </t>
+    <t xml:space="preserve">Canada Goose</t>
   </si>
   <si>
     <t xml:space="preserve">Branta canadensis</t>
@@ -808,7 +808,7 @@
     <t xml:space="preserve">Wszyscy gracze dobierają 1 [card] ze stosu.</t>
   </si>
   <si>
-    <t xml:space="preserve">Carolina Chickadee </t>
+    <t xml:space="preserve">Carolina Chickadee</t>
   </si>
   <si>
     <t xml:space="preserve">Poecile carolinensis</t>
@@ -850,7 +850,7 @@
     <t xml:space="preserve">Dziwuszka Czerwonoczelna</t>
   </si>
   <si>
-    <t xml:space="preserve">Cassin's Sparrow </t>
+    <t xml:space="preserve">Cassin's Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Peucaea cassinii</t>
@@ -871,7 +871,7 @@
     <t xml:space="preserve">Wsuń [card] z ręki pod tę kartę. Jeśli to zrobisz, weź 1 [fruit] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cerulean Warbler </t>
+    <t xml:space="preserve">Cerulean Warbler</t>
   </si>
   <si>
     <t xml:space="preserve">Setophaga cerulea</t>
@@ -895,7 +895,7 @@
     <t xml:space="preserve">Te ptaki liczą się podwójnie tylko na potrzeby realizacji celów, ale już nie w przypadku kart bonusowych czy punktów na koniec gry.&lt;br&gt;Jaja na kartach tych ptaków nie liczą się podwójnie na potrzeby realizacji celów zliczających jaja.</t>
   </si>
   <si>
-    <t xml:space="preserve">Chestnut-Collared Longspur </t>
+    <t xml:space="preserve">Chestnut-Collared Longspur</t>
   </si>
   <si>
     <t xml:space="preserve">Calcarius ornatus</t>
@@ -925,7 +925,7 @@
     <t xml:space="preserve">Kominiarczyk Amerykański</t>
   </si>
   <si>
-    <t xml:space="preserve">Chipping Sparrow </t>
+    <t xml:space="preserve">Chipping Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Spizella passerina</t>
@@ -934,7 +934,7 @@
     <t xml:space="preserve">Spizela Białobrewa</t>
   </si>
   <si>
-    <t xml:space="preserve">Clark's Grebe </t>
+    <t xml:space="preserve">Clark's Grebe</t>
   </si>
   <si>
     <t xml:space="preserve">Aechmophorus clarkii</t>
@@ -943,7 +943,7 @@
     <t xml:space="preserve">Perkoz Żółtodzioby</t>
   </si>
   <si>
-    <t xml:space="preserve">Clark's Nutcracker </t>
+    <t xml:space="preserve">Clark's Nutcracker</t>
   </si>
   <si>
     <t xml:space="preserve">Nucifraga columbiana</t>
@@ -1051,7 +1051,7 @@
     <t xml:space="preserve">W przypadku zdolności tego ptaka symbol [star] liczy się jako [cavity].</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Grackle </t>
+    <t xml:space="preserve">Common Grackle</t>
   </si>
   <si>
     <t xml:space="preserve">Quiscalus quiscula</t>
@@ -1096,7 +1096,7 @@
     <t xml:space="preserve">Nur Lodowiec</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Merganser </t>
+    <t xml:space="preserve">Common Merganser</t>
   </si>
   <si>
     <t xml:space="preserve">Mergus merganser</t>
@@ -1120,7 +1120,7 @@
     <t xml:space="preserve">Jeśli zagrany ptak ma zdolność „GDY ZAGRYWASZ”, aktywuje się ona w momencie zagrania.</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Nighthawk </t>
+    <t xml:space="preserve">Common Nighthawk</t>
   </si>
   <si>
     <t xml:space="preserve">Chordeiles minor</t>
@@ -1171,7 +1171,7 @@
     <t xml:space="preserve">Odrzuć do 5 [invertebrate] ze swoich zasobów. Za każdy odrzucony żeton wsuń po 1 [card] ze stosu pod tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Common Yellowthroat </t>
+    <t xml:space="preserve">Common Yellowthroat</t>
   </si>
   <si>
     <t xml:space="preserve">Geothlypis trichas</t>
@@ -1183,7 +1183,7 @@
     <t xml:space="preserve">Dobierz 2 [card]. Jeśli to zrobisz, na koniec tury odrzuć 1 [card] z ręki.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cooper's Hawk </t>
+    <t xml:space="preserve">Cooper's Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Accipiter cooperii</t>
@@ -1225,7 +1225,7 @@
     <t xml:space="preserve">Łuszczyk Czarnogardły</t>
   </si>
   <si>
-    <t xml:space="preserve">Double-Crested Cormorant </t>
+    <t xml:space="preserve">Double-Crested Cormorant</t>
   </si>
   <si>
     <t xml:space="preserve">Phalacrocorax auritus</t>
@@ -1234,7 +1234,7 @@
     <t xml:space="preserve">Kormoran Rogaty</t>
   </si>
   <si>
-    <t xml:space="preserve">Downy Woodpecker </t>
+    <t xml:space="preserve">Downy Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Picoides pubescens</t>
@@ -1294,7 +1294,7 @@
     <t xml:space="preserve">Gdy inny gracz zagrywa ptaka na [forest], weź 1 [invertebrate] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Eastern Phoebe </t>
+    <t xml:space="preserve">Eastern Phoebe</t>
   </si>
   <si>
     <t xml:space="preserve">Sayornis phoebe</t>
@@ -1306,7 +1306,7 @@
     <t xml:space="preserve">Wszyscy gracze otrzymują 1 [invertebrate] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Eastern Screech Owl </t>
+    <t xml:space="preserve">Eastern Screech Owl</t>
   </si>
   <si>
     <t xml:space="preserve">Megascops asio</t>
@@ -1516,7 +1516,7 @@
     <t xml:space="preserve">Dobierz 1 nową kartę bonusową. Następnie weź 1 [die] z karmnika, złóż 1 [egg] na karcie dowolnego ptaka albo dobierz 1 [card].</t>
   </si>
   <si>
-    <t xml:space="preserve">Ferruginous Hawk </t>
+    <t xml:space="preserve">Ferruginous Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Buteo regalis</t>
@@ -1534,7 +1534,7 @@
     <t xml:space="preserve">Wrona Rybożerna</t>
   </si>
   <si>
-    <t xml:space="preserve">Forster's Tern </t>
+    <t xml:space="preserve">Forster's Tern</t>
   </si>
   <si>
     <t xml:space="preserve">Sterna forsteri</t>
@@ -1543,7 +1543,7 @@
     <t xml:space="preserve">Rybitwa Czarnoucha</t>
   </si>
   <si>
-    <t xml:space="preserve">Franklin's Gull </t>
+    <t xml:space="preserve">Franklin's Gull</t>
   </si>
   <si>
     <t xml:space="preserve">Leucophaeus pipixcan</t>
@@ -1582,7 +1582,7 @@
     <t xml:space="preserve">Podejrzyj [card] ze stosu. Jeśli &lt;100 cm, wsuń kartę ofiary pod tę kartę. Jeśli nie spełnia warunku, odrzuć.</t>
   </si>
   <si>
-    <t xml:space="preserve">Grasshopper Sparrow </t>
+    <t xml:space="preserve">Grasshopper Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Ammodramus savannarum</t>
@@ -1618,7 +1618,7 @@
     <t xml:space="preserve">Zagraj drugiego ptaka na [wetland]. Zapłać jego standardowy koszt.</t>
   </si>
   <si>
-    <t xml:space="preserve">Great Crested Flycatcher </t>
+    <t xml:space="preserve">Great Crested Flycatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Myiarchus crinitus</t>
@@ -1654,7 +1654,7 @@
     <t xml:space="preserve">Czapla Biała</t>
   </si>
   <si>
-    <t xml:space="preserve">Great Horned Owl </t>
+    <t xml:space="preserve">Great Horned Owl</t>
   </si>
   <si>
     <t xml:space="preserve">Bubo virginianus</t>
@@ -1690,7 +1690,7 @@
     <t xml:space="preserve">Możesz wsunąć maksymalnie tyle kart, ile wynosi liczba kostek akcji wybranego gracza w danym siedlisku.</t>
   </si>
   <si>
-    <t xml:space="preserve">Greater Prairie Chicken </t>
+    <t xml:space="preserve">Greater Prairie Chicken</t>
   </si>
   <si>
     <t xml:space="preserve">Tympanuchus cupido</t>
@@ -1699,7 +1699,7 @@
     <t xml:space="preserve">Preriokur Dwuczuby</t>
   </si>
   <si>
-    <t xml:space="preserve">Greater Roadrunner </t>
+    <t xml:space="preserve">Greater Roadrunner</t>
   </si>
   <si>
     <t xml:space="preserve">Geococcyx californianus</t>
@@ -1870,7 +1870,7 @@
     <t xml:space="preserve">Połóż 1 [egg] na każdej swojej karcie ptaka z gniazdem [platform].</t>
   </si>
   <si>
-    <t xml:space="preserve">Indigo Bunting </t>
+    <t xml:space="preserve">Indigo Bunting</t>
   </si>
   <si>
     <t xml:space="preserve">Passerina cyanea</t>
@@ -1882,7 +1882,7 @@
     <t xml:space="preserve">Weź 1 [invertebrate] albo [fruit] z karmnika (jeśli są dostępne).</t>
   </si>
   <si>
-    <t xml:space="preserve">Juniper Titmouse </t>
+    <t xml:space="preserve">Juniper Titmouse</t>
   </si>
   <si>
     <t xml:space="preserve">Baeolophus ridgwayi</t>
@@ -1909,7 +1909,7 @@
     <t xml:space="preserve">Wodnik Królewski</t>
   </si>
   <si>
-    <t xml:space="preserve">Lazuli Bunting </t>
+    <t xml:space="preserve">Lazuli Bunting</t>
   </si>
   <si>
     <t xml:space="preserve">Passerina amoena</t>
@@ -2032,7 +2032,7 @@
     <t xml:space="preserve">Błotniak Łąkowy</t>
   </si>
   <si>
-    <t xml:space="preserve">Mountain Bluebird </t>
+    <t xml:space="preserve">Mountain Bluebird</t>
   </si>
   <si>
     <t xml:space="preserve">Sialia currucoides</t>
@@ -2041,7 +2041,7 @@
     <t xml:space="preserve">Błękitnik Górski</t>
   </si>
   <si>
-    <t xml:space="preserve">Mountain Chickadee </t>
+    <t xml:space="preserve">Mountain Chickadee</t>
   </si>
   <si>
     <t xml:space="preserve">Poecile gambeli</t>
@@ -2050,7 +2050,7 @@
     <t xml:space="preserve">Sikora Górska</t>
   </si>
   <si>
-    <t xml:space="preserve">Mourning Dove </t>
+    <t xml:space="preserve">Mourning Dove</t>
   </si>
   <si>
     <t xml:space="preserve">Zenaida macroura</t>
@@ -2083,7 +2083,7 @@
     <t xml:space="preserve">Przepiór Wirginijski</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Cardinal </t>
+    <t xml:space="preserve">Northern Cardinal</t>
   </si>
   <si>
     <t xml:space="preserve">Cardinalis cardinalis</t>
@@ -2125,7 +2125,7 @@
     <t xml:space="preserve">Jastrząb Zwyczajny</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Harrier </t>
+    <t xml:space="preserve">Northern Harrier</t>
   </si>
   <si>
     <t xml:space="preserve">Circus cyaneus</t>
@@ -2134,7 +2134,7 @@
     <t xml:space="preserve">Błotniak Zbożowy</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Mockingbird </t>
+    <t xml:space="preserve">Northern Mockingbird</t>
   </si>
   <si>
     <t xml:space="preserve">Mimus polyglottos</t>
@@ -2143,7 +2143,7 @@
     <t xml:space="preserve">Przedrzeźniacz Północny</t>
   </si>
   <si>
-    <t xml:space="preserve">Northern Shoveler </t>
+    <t xml:space="preserve">Northern Shoveler</t>
   </si>
   <si>
     <t xml:space="preserve">Spatula clypeata</t>
@@ -2167,7 +2167,7 @@
     <t xml:space="preserve">Wszyscy gracze otrzymują 1 [fish] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Painted Bunting </t>
+    <t xml:space="preserve">Painted Bunting</t>
   </si>
   <si>
     <t xml:space="preserve">Passerina ciris</t>
@@ -2200,7 +2200,7 @@
     <t xml:space="preserve">Otrzymujesz [seed] bez względu na to, jaką kość pożywienia usunąłeś z karmnika.</t>
   </si>
   <si>
-    <t xml:space="preserve">Peregrine Falcon </t>
+    <t xml:space="preserve">Peregrine Falcon</t>
   </si>
   <si>
     <t xml:space="preserve">Falco peregrinus</t>
@@ -2209,7 +2209,7 @@
     <t xml:space="preserve">Sokół Wędrowny</t>
   </si>
   <si>
-    <t xml:space="preserve">Pied-Billed Grebe </t>
+    <t xml:space="preserve">Pied-Billed Grebe</t>
   </si>
   <si>
     <t xml:space="preserve">Podilymbus podiceps</t>
@@ -2218,7 +2218,7 @@
     <t xml:space="preserve">Perkoz Grubodzioby</t>
   </si>
   <si>
-    <t xml:space="preserve">Pileated Woodpecker </t>
+    <t xml:space="preserve">Pileated Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Dryocopus pileatus</t>
@@ -2248,7 +2248,7 @@
     <t xml:space="preserve">Bursztynka</t>
   </si>
   <si>
-    <t xml:space="preserve">Purple Gallinule </t>
+    <t xml:space="preserve">Purple Gallinule</t>
   </si>
   <si>
     <t xml:space="preserve">Porphyrio martinicus</t>
@@ -2320,7 +2320,7 @@
     <t xml:space="preserve">Zabierz 1 [invertebrate] z zasobów innego gracza i przechowaj na tej karcie. Ten gracz bierze 1 [die] z karmnika.</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Bellied Woodpecker </t>
+    <t xml:space="preserve">Red-Bellied Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Melanerpes carolinus</t>
@@ -2338,7 +2338,7 @@
     <t xml:space="preserve">Szlachar</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Breasted Nuthatch </t>
+    <t xml:space="preserve">Red-Breasted Nuthatch</t>
   </si>
   <si>
     <t xml:space="preserve">Sitta canadensis</t>
@@ -2347,7 +2347,7 @@
     <t xml:space="preserve">Kowalik Czarnogłowy</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Cockaded Woodpecker </t>
+    <t xml:space="preserve">Red-Cockaded Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Picoides borealis</t>
@@ -2356,7 +2356,7 @@
     <t xml:space="preserve">Dzięcioł Skromny</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Eyed Vireo </t>
+    <t xml:space="preserve">Red-Eyed Vireo</t>
   </si>
   <si>
     <t xml:space="preserve">Vireo olivaceus</t>
@@ -2365,7 +2365,7 @@
     <t xml:space="preserve">Wireonek Czerwonooki</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Headed Woodpecker </t>
+    <t xml:space="preserve">Red-Headed Woodpecker</t>
   </si>
   <si>
     <t xml:space="preserve">Melanerpes erythrocephalus</t>
@@ -2386,7 +2386,7 @@
     <t xml:space="preserve">Złóż 1 [egg] na każdej karcie ptaka w tej kolumnie, włączając tę kartę.</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Shouldered Hawk </t>
+    <t xml:space="preserve">Red-Shouldered Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Buteo lineatus</t>
@@ -2395,7 +2395,7 @@
     <t xml:space="preserve">Myszołów Rdzawoskrzydły</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Tailed Hawk </t>
+    <t xml:space="preserve">Red-Tailed Hawk</t>
   </si>
   <si>
     <t xml:space="preserve">Buteo jamaicensis</t>
@@ -2404,7 +2404,7 @@
     <t xml:space="preserve">Myszołów Rdzawosterny</t>
   </si>
   <si>
-    <t xml:space="preserve">Red-Winged Blackbird </t>
+    <t xml:space="preserve">Red-Winged Blackbird</t>
   </si>
   <si>
     <t xml:space="preserve">Agelaius phoeniceus</t>
@@ -2422,7 +2422,7 @@
     <t xml:space="preserve">Mewa Delawarska</t>
   </si>
   <si>
-    <t xml:space="preserve">Rose-Breasted Grosbeak </t>
+    <t xml:space="preserve">Rose-Breasted Grosbeak</t>
   </si>
   <si>
     <t xml:space="preserve">Pheucticus ludovicianus</t>
@@ -2434,7 +2434,7 @@
     <t xml:space="preserve">Weź 1 [seed] albo [fruit] z karmnika (jeśli są dostępne).</t>
   </si>
   <si>
-    <t xml:space="preserve">Roseate Spoonbill </t>
+    <t xml:space="preserve">Roseate Spoonbill</t>
   </si>
   <si>
     <t xml:space="preserve">Platalea ajaja</t>
@@ -2443,7 +2443,7 @@
     <t xml:space="preserve">Warzęcha Różowa</t>
   </si>
   <si>
-    <t xml:space="preserve">Ruby-Crowned Kinglet </t>
+    <t xml:space="preserve">Ruby-Crowned Kinglet</t>
   </si>
   <si>
     <t xml:space="preserve">Regulus calendula</t>
@@ -2491,7 +2491,7 @@
     <t xml:space="preserve">Żuraw Kanadyjski</t>
   </si>
   <si>
-    <t xml:space="preserve">Savannah Sparrow </t>
+    <t xml:space="preserve">Savannah Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Passerculus sandwichensis</t>
@@ -2539,7 +2539,7 @@
     <t xml:space="preserve">Złóż 1 [egg] na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Scissor-Tailed Flycatcher </t>
+    <t xml:space="preserve">Scissor-Tailed Flycatcher</t>
   </si>
   <si>
     <t xml:space="preserve">Tyrannus forficatus</t>
@@ -2572,7 +2572,7 @@
     <t xml:space="preserve">Gdy inny gracz z jakiegokolwiek powodu wsuwa [card], wsuń 1 [card] z ręki pod tę kartę. Następnie dobierz 1 [card] na koniec jego tury.</t>
   </si>
   <si>
-    <t xml:space="preserve">Snowy Egret </t>
+    <t xml:space="preserve">Snowy Egret</t>
   </si>
   <si>
     <t xml:space="preserve">Egretta thula</t>
@@ -2590,7 +2590,7 @@
     <t xml:space="preserve">Puchacz Śnieżny</t>
   </si>
   <si>
-    <t xml:space="preserve">Song Sparrow </t>
+    <t xml:space="preserve">Song Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Melospiza melodia</t>
@@ -2608,7 +2608,7 @@
     <t xml:space="preserve">Puszczyk Plamisty</t>
   </si>
   <si>
-    <t xml:space="preserve">Spotted Sandpiper </t>
+    <t xml:space="preserve">Spotted Sandpiper</t>
   </si>
   <si>
     <t xml:space="preserve">Actitis macularius</t>
@@ -2617,7 +2617,7 @@
     <t xml:space="preserve">Brodziec Plamisty</t>
   </si>
   <si>
-    <t xml:space="preserve">Spotted Towhee </t>
+    <t xml:space="preserve">Spotted Towhee</t>
   </si>
   <si>
     <t xml:space="preserve">Pipilo maculatus</t>
@@ -2680,7 +2680,7 @@
     <t xml:space="preserve">Odrzuć 1 [seed] ze swoich zasobów. Jeśli to zrobisz, złóż 2 [egg] na tej karcie.</t>
   </si>
   <si>
-    <t xml:space="preserve">Tree Swallow </t>
+    <t xml:space="preserve">Tree Swallow</t>
   </si>
   <si>
     <t xml:space="preserve">Tachycineta bicolor</t>
@@ -2728,7 +2728,7 @@
     <t xml:space="preserve">Wsuń [card] z ręki pod tę kartę. Jeśli to zrobisz, weź 1 [invertebrate] z zasobów.</t>
   </si>
   <si>
-    <t xml:space="preserve">Violet-Green Swallow </t>
+    <t xml:space="preserve">Violet-Green Swallow</t>
   </si>
   <si>
     <t xml:space="preserve">Tachycineta thalassina</t>
@@ -2791,7 +2791,7 @@
     <t xml:space="preserve">Jeśli wszystkie kości w karmniku wskazują ten sam symbol, możesz go opróżnić i ponownie napełnić przed pobraniem [die].</t>
   </si>
   <si>
-    <t xml:space="preserve">White-Breasted Nuthatch </t>
+    <t xml:space="preserve">White-Breasted Nuthatch</t>
   </si>
   <si>
     <t xml:space="preserve">Sitta carolinensis</t>
@@ -2800,7 +2800,7 @@
     <t xml:space="preserve">Kowalik Karoliński</t>
   </si>
   <si>
-    <t xml:space="preserve">White-Crowned Sparrow </t>
+    <t xml:space="preserve">White-Crowned Sparrow</t>
   </si>
   <si>
     <t xml:space="preserve">Zonotrichia leucophrys</t>
@@ -2809,7 +2809,7 @@
     <t xml:space="preserve">Pasówka Białobrewa</t>
   </si>
   <si>
-    <t xml:space="preserve">White-Faced Ibis </t>
+    <t xml:space="preserve">White-Faced Ibis</t>
   </si>
   <si>
     <t xml:space="preserve">Plegadis chihi</t>
@@ -2902,7 +2902,7 @@
     <t xml:space="preserve">Dławigad Amerykański</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Bellied Sapsucker </t>
+    <t xml:space="preserve">Yellow-Bellied Sapsucker</t>
   </si>
   <si>
     <t xml:space="preserve">Sphyrapicus varius</t>
@@ -2920,7 +2920,7 @@
     <t xml:space="preserve">Kukawik Żółtodzioby</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Breasted Chat </t>
+    <t xml:space="preserve">Yellow-Breasted Chat</t>
   </si>
   <si>
     <t xml:space="preserve">Icteria virens</t>
@@ -2929,7 +2929,7 @@
     <t xml:space="preserve">Słowikówka</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Headed Blackbird </t>
+    <t xml:space="preserve">Yellow-Headed Blackbird</t>
   </si>
   <si>
     <t xml:space="preserve">Xanthocephalus xanthocephalus</t>
@@ -2938,7 +2938,7 @@
     <t xml:space="preserve">Żółtogłowiec</t>
   </si>
   <si>
-    <t xml:space="preserve">Yellow-Rumped Warbler </t>
+    <t xml:space="preserve">Yellow-Rumped Warbler</t>
   </si>
   <si>
     <t xml:space="preserve">Setophaga coronata</t>
@@ -6031,30 +6031,6 @@
     <t xml:space="preserve">Szereg ptaków w [wetland] o rosnącej albo malejącej rozpiętości skrzydeł.</t>
   </si>
   <si>
-    <t xml:space="preserve">[automa] Avid Asian Avian Admirer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[automa] Zagorzały miłośnik ptaków azjatyckich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;2&lt;/b&gt; albo &lt;b&gt;3&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;3&lt;/b&gt; albo &lt;b&gt;4&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt; albo &lt;b&gt;5&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Zaczyna od kart z niższą wartością).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[automa] Rare Species Lister</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[automa] Znawca rzadkich gatunków</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt;, &lt;b&gt;5&lt;/b&gt; albo &lt;b&gt;6&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;5&lt;/b&gt;, &lt;b&gt;6&lt;/b&gt; albo &lt;b&gt;7&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;6&lt;/b&gt;, &lt;b&gt;7&lt;/b&gt; albo &lt;b&gt;8&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Automa zatrzymuje kartę o najniższej wartości.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Avian Theriogenologist</t>
   </si>
   <si>
@@ -6273,6 +6249,30 @@
   </si>
   <si>
     <t xml:space="preserve">Policz, ile niewykorzystanych żetonów pożywienia masz na koniec gry w swoich zasobach. Pożywienie przechowywane na kartach ptaków nie liczy się jako część zasobów.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Avid Asian Avian Admirer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Zagorzały miłośnik ptaków azjatyckich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;2&lt;/b&gt; albo &lt;b&gt;3&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;3&lt;/b&gt; albo &lt;b&gt;4&lt;/b&gt; punkty&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt; albo &lt;b&gt;5&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Zaczyna od kart z niższą wartością).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Rare Species Lister</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[automa] Znawca rzadkich gatunków</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;table&gt;&lt;th&gt;Poziom trudności&lt;/th&gt;&lt;th&gt;Ptaki warte&lt;/th&gt;&lt;tr&gt;&lt;td&gt;Orlę&lt;/td&gt;&lt;td&gt;&lt;b&gt;4&lt;/b&gt;, &lt;b&gt;5&lt;/b&gt; albo &lt;b&gt;6&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;5&lt;/b&gt;, &lt;b&gt;6&lt;/b&gt; albo &lt;b&gt;7&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td&gt;Szybujący orzeł&lt;/td&gt;&lt;td&gt;&lt;b&gt;6&lt;/b&gt;, &lt;b&gt;7&lt;/b&gt; albo &lt;b&gt;8&lt;/b&gt; punktów&lt;/td&gt;&lt;/tr&gt;&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automa zatrzymuje kartę o najniższej wartości.</t>
   </si>
   <si>
     <t xml:space="preserve">Translated</t>
@@ -6507,7 +6507,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6515,7 +6515,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6568,6 +6568,112 @@
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -6575,8 +6681,10 @@
   </sheetPr>
   <dimension ref="A1:K447"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="C271" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G271" activeCellId="0" sqref="G271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18824,7 +18932,7 @@
       <c r="J433" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K433" s="0" t="s">
+      <c r="K433" s="1" t="s">
         <v>22</v>
       </c>
     </row>
@@ -19255,8 +19363,10 @@
   </sheetPr>
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F51" activeCellId="0" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19265,7 +19375,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="53.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.88"/>
@@ -20227,7 +20337,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
-        <v>1050</v>
+        <v>1039</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>1956</v>
@@ -20235,166 +20345,169 @@
       <c r="C40" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="1" t="s">
         <v>1957</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="1" t="s">
         <v>1958</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="1" t="s">
         <v>1959</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>1928</v>
+      <c r="G40" s="9" t="s">
+        <v>1960</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>1961</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
-        <v>1051</v>
+        <v>1040</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>1960</v>
+        <v>1962</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>1961</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>1962</v>
-      </c>
-      <c r="G41" s="4" t="s">
+      <c r="D41" s="1" t="s">
         <v>1963</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>1964</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>1965</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>1966</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>1964</v>
+        <v>1967</v>
       </c>
       <c r="C42" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>1965</v>
+        <v>1968</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>1966</v>
+        <v>1969</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1967</v>
+        <v>1970</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>1968</v>
+        <v>1971</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>1969</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>1970</v>
+        <v>1973</v>
       </c>
       <c r="C43" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1971</v>
+        <v>1974</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>1972</v>
+        <v>1975</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>1973</v>
+        <v>1936</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>1974</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="2" t="n">
-        <v>1041</v>
+      <c r="A44" s="9" t="n">
+        <v>1043</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>1975</v>
+        <v>1977</v>
       </c>
       <c r="C44" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>1976</v>
+        <v>1978</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>1977</v>
+        <v>1979</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1978</v>
+        <v>1970</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>1979</v>
+        <v>1971</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>1980</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>1982</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>1983</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>1936</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>1984</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="n">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="C46" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>1984</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>1985</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>1986</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="H46" s="1" t="s">
         <v>1987</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>1978</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>1979</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>1980</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>1988</v>
@@ -20408,39 +20521,45 @@
       <c r="E47" s="1" t="s">
         <v>1990</v>
       </c>
+      <c r="F47" s="1" t="s">
+        <v>1991</v>
+      </c>
       <c r="G47" s="9" t="s">
-        <v>1936</v>
+        <v>1818</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>1984</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="9" t="n">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>1991</v>
+        <v>1993</v>
       </c>
       <c r="C48" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>1992</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>1993</v>
+        <v>1994</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>1995</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>1970</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>1994</v>
+        <v>1971</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>1995</v>
+        <v>1972</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>1996</v>
@@ -20454,45 +20573,39 @@
       <c r="E49" s="1" t="s">
         <v>1998</v>
       </c>
-      <c r="F49" s="1" t="s">
-        <v>1999</v>
-      </c>
       <c r="G49" s="9" t="s">
-        <v>1818</v>
+        <v>1936</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>2000</v>
+        <v>1976</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="n">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="C50" s="11" t="s">
         <v>1381</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>2000</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>2002</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>2003</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>1978</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>1979</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>1980</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>2004</v>
@@ -20500,39 +20613,36 @@
       <c r="C51" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="9" t="s">
         <v>2005</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E51" s="9" t="s">
         <v>2006</v>
       </c>
-      <c r="G51" s="9" t="s">
-        <v>1936</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>1984</v>
+      <c r="F51" s="4" t="s">
+        <v>2007</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>1928</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9" t="n">
-        <v>1049</v>
+      <c r="A52" s="2" t="n">
+        <v>1051</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="C52" s="11" t="s">
         <v>1381</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>2008</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="D52" s="9" t="s">
         <v>2009</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="E52" s="9" t="s">
         <v>2010</v>
       </c>
-      <c r="H52" s="1" t="s">
+      <c r="G52" s="4" t="s">
         <v>2011</v>
       </c>
     </row>

</xml_diff>